<commit_message>
commit while first configuring with jenkins
</commit_message>
<xml_diff>
--- a/seleniumTest/src/main/resources/Practice Form.xlsx
+++ b/seleniumTest/src/main/resources/Practice Form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaurav.guleria/git/seleniumTest/seleniumTest/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{EEDD10A6-C0A4-364D-A225-C558B5BE6F88}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{964ECE75-AFEF-C546-9484-86D3B7D43960}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
     <workbookView windowHeight="15440" windowWidth="26440" xWindow="340" xr2:uid="{8DDF1720-135F-A64C-B290-8DC9E33E3B1A}" yWindow="1580"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Browser</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>First Name</t>
   </si>
@@ -87,16 +84,19 @@
     <t>Navigation Commands</t>
   </si>
   <si>
-    <t>Test case executed Successfully</t>
-  </si>
-  <si>
     <t>/src/main/resources/Feb bill.pdf</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>QTP</t>
+  </si>
+  <si>
+    <t>rohit</t>
+  </si>
+  <si>
+    <t>rana</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t/>
@@ -492,19 +492,19 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="7" width="16.5" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.83203125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="9.83203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="41.5" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="7" width="16.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="41.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,10 +514,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -530,18 +530,15 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -549,36 +546,62 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44257</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3">
-        <v>44257</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44278</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>